<commit_message>
Added new pictures for 4.2
</commit_message>
<xml_diff>
--- a/pics/ue4/Details_Atom_Y-Histogramm.xlsx
+++ b/pics/ue4/Details_Atom_Y-Histogramm.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tobias\Desktop\Mt\pics\ue4\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="28515" windowHeight="12585"/>
   </bookViews>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -70,12 +75,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -906,6 +914,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-573E-405A-957F-8CA29E146011}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -932,757 +945,757 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>71</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>85</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>146</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>330</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>387</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>401</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>459</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>471</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>392</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>462</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>397</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>390</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>517</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>734</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1593</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3667</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6155</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>6552</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4078</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2434</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2009</c:v>
-                </c:pt>
                 <c:pt idx="25">
-                  <c:v>2163</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2465</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2887</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3075</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3360</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3207</c:v>
+                  <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2840</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3327</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3699</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3600</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4351</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4503</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5519</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5323</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4148</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3965</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3914</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4051</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4016</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3792</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>5325</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5223</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4893</c:v>
+                  <c:v>153</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>5657</c:v>
+                  <c:v>186</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>7685</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>20050</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>31222</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>24199</c:v>
+                  <c:v>245</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>15188</c:v>
+                  <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>16924</c:v>
+                  <c:v>426</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>21036</c:v>
+                  <c:v>522</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>35656</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>12315</c:v>
+                  <c:v>888</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>8797</c:v>
+                  <c:v>1219</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>9259</c:v>
+                  <c:v>1560</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>8722</c:v>
+                  <c:v>1930</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>17662</c:v>
+                  <c:v>2042</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>23254</c:v>
+                  <c:v>2184</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>28849</c:v>
+                  <c:v>2351</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>30707</c:v>
+                  <c:v>2250</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>11125</c:v>
+                  <c:v>1953</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4187</c:v>
+                  <c:v>1550</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4859</c:v>
+                  <c:v>1396</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>4149</c:v>
+                  <c:v>1130</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>4453</c:v>
+                  <c:v>861</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>4159</c:v>
+                  <c:v>785</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>3593</c:v>
+                  <c:v>792</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>4844</c:v>
+                  <c:v>728</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>5426</c:v>
+                  <c:v>678</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>6030</c:v>
+                  <c:v>597</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>5072</c:v>
+                  <c:v>706</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>4046</c:v>
+                  <c:v>793</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>3512</c:v>
+                  <c:v>665</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>2967</c:v>
+                  <c:v>668</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1588</c:v>
+                  <c:v>853</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>2473</c:v>
+                  <c:v>947</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>2439</c:v>
+                  <c:v>951</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>3076</c:v>
+                  <c:v>878</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1545</c:v>
+                  <c:v>1059</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0</c:v>
+                  <c:v>1175</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0</c:v>
+                  <c:v>873</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0</c:v>
+                  <c:v>1131</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0</c:v>
+                  <c:v>1235</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0</c:v>
+                  <c:v>995</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0</c:v>
+                  <c:v>878</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0</c:v>
+                  <c:v>1202</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0</c:v>
+                  <c:v>1126</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0</c:v>
+                  <c:v>944</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0</c:v>
+                  <c:v>807</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0</c:v>
+                  <c:v>1089</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0</c:v>
+                  <c:v>1292</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0</c:v>
+                  <c:v>1028</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0</c:v>
+                  <c:v>1012</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0</c:v>
+                  <c:v>1266</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0</c:v>
+                  <c:v>1256</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>0</c:v>
+                  <c:v>1171</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>0</c:v>
+                  <c:v>929</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>0</c:v>
+                  <c:v>1209</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>0</c:v>
+                  <c:v>1465</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>0</c:v>
+                  <c:v>1334</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>0</c:v>
+                  <c:v>1330</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>0</c:v>
+                  <c:v>1696</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>0</c:v>
+                  <c:v>1650</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>0</c:v>
+                  <c:v>1522</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>0</c:v>
+                  <c:v>1322</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>0</c:v>
+                  <c:v>1694</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>0</c:v>
+                  <c:v>1926</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>0</c:v>
+                  <c:v>1897</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>0</c:v>
+                  <c:v>1799</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>0</c:v>
+                  <c:v>1830</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>0</c:v>
+                  <c:v>1693</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>0</c:v>
+                  <c:v>1490</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>0</c:v>
+                  <c:v>1231</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>0</c:v>
+                  <c:v>1428</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>0</c:v>
+                  <c:v>1551</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>0</c:v>
+                  <c:v>1237</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>0</c:v>
+                  <c:v>1176</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>0</c:v>
+                  <c:v>1336</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>0</c:v>
+                  <c:v>1370</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>0</c:v>
+                  <c:v>1207</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>0</c:v>
+                  <c:v>1026</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>0</c:v>
+                  <c:v>1395</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>0</c:v>
+                  <c:v>1632</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>0</c:v>
+                  <c:v>1474</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>0</c:v>
+                  <c:v>1235</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>0</c:v>
+                  <c:v>1310</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>0</c:v>
+                  <c:v>1373</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>0</c:v>
+                  <c:v>1265</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>0</c:v>
+                  <c:v>1149</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>0</c:v>
+                  <c:v>1459</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>0</c:v>
+                  <c:v>2062</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>0</c:v>
+                  <c:v>1806</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>0</c:v>
+                  <c:v>1626</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>0</c:v>
+                  <c:v>1757</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>0</c:v>
+                  <c:v>1842</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>0</c:v>
+                  <c:v>1663</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>0</c:v>
+                  <c:v>1530</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>0</c:v>
+                  <c:v>1703</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>0</c:v>
+                  <c:v>2049</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>0</c:v>
+                  <c:v>1842</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>0</c:v>
+                  <c:v>1766</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>0</c:v>
+                  <c:v>2039</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>0</c:v>
+                  <c:v>2441</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>0</c:v>
+                  <c:v>3210</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>0</c:v>
+                  <c:v>3701</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>0</c:v>
+                  <c:v>6433</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>0</c:v>
+                  <c:v>9919</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>0</c:v>
+                  <c:v>9626</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>0</c:v>
+                  <c:v>10036</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>0</c:v>
+                  <c:v>11557</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>0</c:v>
+                  <c:v>11431</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>0</c:v>
+                  <c:v>7897</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>0</c:v>
+                  <c:v>4868</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>0</c:v>
+                  <c:v>4303</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>0</c:v>
+                  <c:v>5564</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>0</c:v>
+                  <c:v>5320</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>0</c:v>
+                  <c:v>5154</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>0</c:v>
+                  <c:v>5758</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>0</c:v>
+                  <c:v>6013</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>0</c:v>
+                  <c:v>5488</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>0</c:v>
+                  <c:v>5423</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>0</c:v>
+                  <c:v>10126</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>0</c:v>
+                  <c:v>16970</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>0</c:v>
+                  <c:v>11565</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>0</c:v>
+                  <c:v>7117</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>0</c:v>
+                  <c:v>5290</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>0</c:v>
+                  <c:v>4269</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>0</c:v>
+                  <c:v>2753</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>0</c:v>
+                  <c:v>2139</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>0</c:v>
+                  <c:v>2709</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>0</c:v>
+                  <c:v>3954</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>0</c:v>
+                  <c:v>3355</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>0</c:v>
+                  <c:v>3019</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>0</c:v>
+                  <c:v>2900</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>0</c:v>
+                  <c:v>3034</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>0</c:v>
+                  <c:v>2960</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>0</c:v>
+                  <c:v>2713</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>0</c:v>
+                  <c:v>4206</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>0</c:v>
+                  <c:v>6949</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>0</c:v>
+                  <c:v>6520</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>0</c:v>
+                  <c:v>6380</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>0</c:v>
+                  <c:v>7850</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>0</c:v>
+                  <c:v>9037</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>0</c:v>
+                  <c:v>9317</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>0</c:v>
+                  <c:v>8621</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>0</c:v>
+                  <c:v>11134</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>0</c:v>
+                  <c:v>14775</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>0</c:v>
+                  <c:v>8760</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>0</c:v>
+                  <c:v>6943</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>0</c:v>
+                  <c:v>5605</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>0</c:v>
+                  <c:v>3929</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>0</c:v>
+                  <c:v>1565</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>0</c:v>
+                  <c:v>1050</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>0</c:v>
+                  <c:v>1278</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>0</c:v>
+                  <c:v>1858</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>0</c:v>
+                  <c:v>1515</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>0</c:v>
+                  <c:v>1557</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>0</c:v>
+                  <c:v>1786</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>0</c:v>
+                  <c:v>1750</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>0</c:v>
+                  <c:v>1414</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>0</c:v>
+                  <c:v>985</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>0</c:v>
+                  <c:v>1302</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>0</c:v>
+                  <c:v>1840</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>0</c:v>
+                  <c:v>1311</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>0</c:v>
+                  <c:v>1258</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>0</c:v>
+                  <c:v>1332</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>0</c:v>
+                  <c:v>1569</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>0</c:v>
+                  <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>0</c:v>
+                  <c:v>1037</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>0</c:v>
+                  <c:v>1257</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>0</c:v>
+                  <c:v>1919</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>0</c:v>
+                  <c:v>1561</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>0</c:v>
+                  <c:v>1364</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>0</c:v>
+                  <c:v>1746</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>0</c:v>
+                  <c:v>2008</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>0</c:v>
+                  <c:v>1676</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>0</c:v>
+                  <c:v>1282</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>0</c:v>
+                  <c:v>1846</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>0</c:v>
+                  <c:v>2898</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>0</c:v>
+                  <c:v>1847</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>0</c:v>
+                  <c:v>1541</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>0</c:v>
+                  <c:v>1683</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>0</c:v>
+                  <c:v>1823</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>0</c:v>
+                  <c:v>1254</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>0</c:v>
+                  <c:v>969</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>0</c:v>
+                  <c:v>953</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>0</c:v>
+                  <c:v>1523</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>0</c:v>
+                  <c:v>1036</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>0</c:v>
+                  <c:v>960</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>0</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>0</c:v>
+                  <c:v>1007</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>0</c:v>
+                  <c:v>616</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>0</c:v>
+                  <c:v>438</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>0</c:v>
+                  <c:v>534</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>0</c:v>
+                  <c:v>993</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>0</c:v>
+                  <c:v>766</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>0</c:v>
+                  <c:v>714</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>0</c:v>
+                  <c:v>810</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>0</c:v>
+                  <c:v>873</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>0</c:v>
+                  <c:v>756</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>0</c:v>
+                  <c:v>609</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>0</c:v>
+                  <c:v>958</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>0</c:v>
+                  <c:v>1509</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>0</c:v>
+                  <c:v>948</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>0</c:v>
+                  <c:v>561</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="252">
                   <c:v>0</c:v>
@@ -1699,9 +1712,13 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-573E-405A-957F-8CA29E146011}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1815,13 +1832,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -1858,9 +1875,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1898,9 +1915,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1935,7 +1952,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1970,7 +1987,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2146,16 +2163,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2163,2051 +2179,2051 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="1">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="1">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="1">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="1">
-        <v>1593</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="1">
-        <v>3667</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="1">
-        <v>6155</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="1">
-        <v>6552</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="1">
-        <v>4078</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="1">
-        <v>2434</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="1">
-        <v>2009</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="1">
-        <v>2163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="1">
-        <v>2465</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="1">
-        <v>2887</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="1">
-        <v>3075</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="1">
-        <v>3360</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="1">
-        <v>3207</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="1">
-        <v>2840</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" s="1">
-        <v>3327</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35" s="1">
-        <v>3699</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36" s="1">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>35</v>
       </c>
-      <c r="B37" s="1">
-        <v>4351</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38" s="1">
-        <v>4503</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" s="1">
-        <v>5519</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" s="1">
-        <v>5323</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="1">
-        <v>4148</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" s="1">
-        <v>3965</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" s="1">
-        <v>3914</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="1">
-        <v>4051</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45" s="1">
-        <v>4016</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>44</v>
       </c>
-      <c r="B46" s="1">
-        <v>3792</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47" s="1">
-        <v>5325</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" s="1">
-        <v>5223</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49" s="1">
-        <v>4893</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50" s="1">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51" s="1">
-        <v>7685</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" s="1">
-        <v>20050</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>51</v>
       </c>
-      <c r="B53" s="1">
-        <v>31222</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>52</v>
       </c>
-      <c r="B54" s="1">
-        <v>24199</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>53</v>
       </c>
-      <c r="B55" s="1">
-        <v>15188</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B56" s="1">
-        <v>16924</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>55</v>
       </c>
-      <c r="B57" s="1">
-        <v>21036</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>56</v>
       </c>
-      <c r="B58" s="1">
-        <v>35656</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>57</v>
       </c>
-      <c r="B59" s="1">
-        <v>12315</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>58</v>
       </c>
-      <c r="B60" s="1">
-        <v>8797</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>59</v>
       </c>
-      <c r="B61" s="1">
-        <v>9259</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62" s="1">
-        <v>8722</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63" s="1">
-        <v>17662</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B64" s="1">
-        <v>23254</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>2184</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B65" s="1">
-        <v>28849</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>2351</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66" s="1">
-        <v>30707</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B67" s="1">
-        <v>11125</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B68" s="1">
-        <v>4187</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>67</v>
       </c>
-      <c r="B69" s="1">
-        <v>4859</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>68</v>
       </c>
-      <c r="B70" s="1">
-        <v>4149</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71" s="1">
-        <v>4453</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>70</v>
       </c>
-      <c r="B72" s="1">
-        <v>4159</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>71</v>
       </c>
-      <c r="B73" s="1">
-        <v>3593</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>72</v>
       </c>
-      <c r="B74" s="1">
-        <v>4844</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>73</v>
       </c>
-      <c r="B75" s="1">
-        <v>5426</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>74</v>
       </c>
-      <c r="B76" s="1">
-        <v>6030</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>75</v>
       </c>
-      <c r="B77" s="1">
-        <v>5072</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>76</v>
       </c>
-      <c r="B78" s="1">
-        <v>4046</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>77</v>
       </c>
-      <c r="B79" s="1">
-        <v>3512</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>78</v>
       </c>
-      <c r="B80" s="1">
-        <v>2967</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>79</v>
       </c>
-      <c r="B81" s="1">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>80</v>
       </c>
-      <c r="B82" s="1">
-        <v>2473</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>81</v>
       </c>
-      <c r="B83" s="1">
-        <v>2439</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>82</v>
       </c>
-      <c r="B84" s="1">
-        <v>3076</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>83</v>
       </c>
-      <c r="B85" s="1">
-        <v>1545</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>84</v>
       </c>
-      <c r="B86" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>85</v>
       </c>
-      <c r="B87" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>86</v>
       </c>
-      <c r="B88" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>87</v>
       </c>
-      <c r="B89" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>88</v>
       </c>
-      <c r="B90" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>89</v>
       </c>
-      <c r="B91" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>90</v>
       </c>
-      <c r="B92" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>91</v>
       </c>
-      <c r="B93" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>92</v>
       </c>
-      <c r="B94" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>93</v>
       </c>
-      <c r="B95" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>94</v>
       </c>
-      <c r="B96" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>95</v>
       </c>
-      <c r="B97" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>96</v>
       </c>
-      <c r="B98" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>97</v>
       </c>
-      <c r="B99" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>98</v>
       </c>
-      <c r="B100" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A101" s="1">
         <v>99</v>
       </c>
-      <c r="B101" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A102" s="1">
         <v>100</v>
       </c>
-      <c r="B102" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A103" s="1">
         <v>101</v>
       </c>
-      <c r="B103" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A104" s="1">
         <v>102</v>
       </c>
-      <c r="B104" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A105" s="1">
         <v>103</v>
       </c>
-      <c r="B105" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A106" s="1">
         <v>104</v>
       </c>
-      <c r="B106" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A107" s="1">
         <v>105</v>
       </c>
-      <c r="B107" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A108" s="1">
         <v>106</v>
       </c>
-      <c r="B108" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A109" s="1">
         <v>107</v>
       </c>
-      <c r="B109" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A110" s="1">
         <v>108</v>
       </c>
-      <c r="B110" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A111" s="1">
         <v>109</v>
       </c>
-      <c r="B111" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A112" s="1">
         <v>110</v>
       </c>
-      <c r="B112" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A113" s="1">
         <v>111</v>
       </c>
-      <c r="B113" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A114" s="1">
         <v>112</v>
       </c>
-      <c r="B114" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A115" s="1">
         <v>113</v>
       </c>
-      <c r="B115" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A116" s="1">
         <v>114</v>
       </c>
-      <c r="B116" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A117" s="1">
         <v>115</v>
       </c>
-      <c r="B117" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A118" s="1">
         <v>116</v>
       </c>
-      <c r="B118" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A119" s="1">
         <v>117</v>
       </c>
-      <c r="B119" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A120" s="1">
         <v>118</v>
       </c>
-      <c r="B120" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A121" s="1">
         <v>119</v>
       </c>
-      <c r="B121" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A122" s="1">
         <v>120</v>
       </c>
-      <c r="B122" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A123" s="1">
         <v>121</v>
       </c>
-      <c r="B123" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A124" s="1">
         <v>122</v>
       </c>
-      <c r="B124" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A125" s="1">
         <v>123</v>
       </c>
-      <c r="B125" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A126" s="1">
         <v>124</v>
       </c>
-      <c r="B126" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A127" s="1">
         <v>125</v>
       </c>
-      <c r="B127" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A128" s="1">
         <v>126</v>
       </c>
-      <c r="B128" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A129" s="1">
         <v>127</v>
       </c>
-      <c r="B129" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A130" s="1">
         <v>128</v>
       </c>
-      <c r="B130" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A131" s="1">
         <v>129</v>
       </c>
-      <c r="B131" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A132" s="1">
         <v>130</v>
       </c>
-      <c r="B132" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A133" s="1">
         <v>131</v>
       </c>
-      <c r="B133" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A134" s="1">
         <v>132</v>
       </c>
-      <c r="B134" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A135" s="1">
         <v>133</v>
       </c>
-      <c r="B135" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A136" s="1">
         <v>134</v>
       </c>
-      <c r="B136" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A137" s="1">
         <v>135</v>
       </c>
-      <c r="B137" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A138" s="1">
         <v>136</v>
       </c>
-      <c r="B138" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>2062</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A139" s="1">
         <v>137</v>
       </c>
-      <c r="B139" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A140" s="1">
         <v>138</v>
       </c>
-      <c r="B140" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A141" s="1">
         <v>139</v>
       </c>
-      <c r="B141" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A142" s="1">
         <v>140</v>
       </c>
-      <c r="B142" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B142">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A143" s="1">
         <v>141</v>
       </c>
-      <c r="B143" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A144" s="1">
         <v>142</v>
       </c>
-      <c r="B144" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B144">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A145" s="1">
         <v>143</v>
       </c>
-      <c r="B145" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A146" s="1">
         <v>144</v>
       </c>
-      <c r="B146" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A147" s="1">
         <v>145</v>
       </c>
-      <c r="B147" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B147">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A148" s="1">
         <v>146</v>
       </c>
-      <c r="B148" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B148">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A149" s="1">
         <v>147</v>
       </c>
-      <c r="B149" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B149">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A150" s="1">
         <v>148</v>
       </c>
-      <c r="B150" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>2441</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A151" s="1">
         <v>149</v>
       </c>
-      <c r="B151" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B151">
+        <v>3210</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A152" s="1">
         <v>150</v>
       </c>
-      <c r="B152" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B152">
+        <v>3701</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A153" s="1">
         <v>151</v>
       </c>
-      <c r="B153" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>6433</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A154" s="1">
         <v>152</v>
       </c>
-      <c r="B154" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B154">
+        <v>9919</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A155" s="1">
         <v>153</v>
       </c>
-      <c r="B155" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B155">
+        <v>9626</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A156" s="1">
         <v>154</v>
       </c>
-      <c r="B156" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B156">
+        <v>10036</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A157" s="1">
         <v>155</v>
       </c>
-      <c r="B157" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>11557</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A158" s="1">
         <v>156</v>
       </c>
-      <c r="B158" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B158">
+        <v>11431</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A159" s="1">
         <v>157</v>
       </c>
-      <c r="B159" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>7897</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A160" s="1">
         <v>158</v>
       </c>
-      <c r="B160" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B160">
+        <v>4868</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A161" s="1">
         <v>159</v>
       </c>
-      <c r="B161" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>4303</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A162" s="1">
         <v>160</v>
       </c>
-      <c r="B162" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>5564</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A163" s="1">
         <v>161</v>
       </c>
-      <c r="B163" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>5320</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A164" s="1">
         <v>162</v>
       </c>
-      <c r="B164" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B164">
+        <v>5154</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A165" s="1">
         <v>163</v>
       </c>
-      <c r="B165" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>5758</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A166" s="1">
         <v>164</v>
       </c>
-      <c r="B166" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B166">
+        <v>6013</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A167" s="1">
         <v>165</v>
       </c>
-      <c r="B167" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <v>5488</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A168" s="1">
         <v>166</v>
       </c>
-      <c r="B168" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B168">
+        <v>5423</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A169" s="1">
         <v>167</v>
       </c>
-      <c r="B169" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>10126</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A170" s="1">
         <v>168</v>
       </c>
-      <c r="B170" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B170">
+        <v>16970</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A171" s="1">
         <v>169</v>
       </c>
-      <c r="B171" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B171">
+        <v>11565</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A172" s="1">
         <v>170</v>
       </c>
-      <c r="B172" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B172">
+        <v>7117</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A173" s="1">
         <v>171</v>
       </c>
-      <c r="B173" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B173">
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A174" s="1">
         <v>172</v>
       </c>
-      <c r="B174" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B174">
+        <v>4269</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A175" s="1">
         <v>173</v>
       </c>
-      <c r="B175" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B175">
+        <v>2753</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A176" s="1">
         <v>174</v>
       </c>
-      <c r="B176" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <v>2139</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A177" s="1">
         <v>175</v>
       </c>
-      <c r="B177" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B177">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A178" s="1">
         <v>176</v>
       </c>
-      <c r="B178" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B178">
+        <v>3954</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A179" s="1">
         <v>177</v>
       </c>
-      <c r="B179" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B179">
+        <v>3355</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A180" s="1">
         <v>178</v>
       </c>
-      <c r="B180" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B180">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A181" s="1">
         <v>179</v>
       </c>
-      <c r="B181" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B181">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A182" s="1">
         <v>180</v>
       </c>
-      <c r="B182" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B182">
+        <v>3034</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A183" s="1">
         <v>181</v>
       </c>
-      <c r="B183" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B183">
+        <v>2960</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A184" s="1">
         <v>182</v>
       </c>
-      <c r="B184" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B184">
+        <v>2713</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A185" s="1">
         <v>183</v>
       </c>
-      <c r="B185" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B185">
+        <v>4206</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A186" s="1">
         <v>184</v>
       </c>
-      <c r="B186" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B186">
+        <v>6949</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A187" s="1">
         <v>185</v>
       </c>
-      <c r="B187" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B187">
+        <v>6520</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A188" s="1">
         <v>186</v>
       </c>
-      <c r="B188" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B188">
+        <v>6380</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A189" s="1">
         <v>187</v>
       </c>
-      <c r="B189" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B189">
+        <v>7850</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A190" s="1">
         <v>188</v>
       </c>
-      <c r="B190" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B190">
+        <v>9037</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A191" s="1">
         <v>189</v>
       </c>
-      <c r="B191" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B191">
+        <v>9317</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A192" s="1">
         <v>190</v>
       </c>
-      <c r="B192" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <v>8621</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A193" s="1">
         <v>191</v>
       </c>
-      <c r="B193" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B193">
+        <v>11134</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A194" s="1">
         <v>192</v>
       </c>
-      <c r="B194" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B194">
+        <v>14775</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A195" s="1">
         <v>193</v>
       </c>
-      <c r="B195" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B195">
+        <v>8760</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A196" s="1">
         <v>194</v>
       </c>
-      <c r="B196" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B196">
+        <v>6943</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A197" s="1">
         <v>195</v>
       </c>
-      <c r="B197" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B197">
+        <v>5605</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A198" s="1">
         <v>196</v>
       </c>
-      <c r="B198" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B198">
+        <v>3929</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A199" s="1">
         <v>197</v>
       </c>
-      <c r="B199" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B199">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A200" s="1">
         <v>198</v>
       </c>
-      <c r="B200" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B200">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A201" s="1">
         <v>199</v>
       </c>
-      <c r="B201" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B201">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A202" s="1">
         <v>200</v>
       </c>
-      <c r="B202" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B202">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A203" s="1">
         <v>201</v>
       </c>
-      <c r="B203" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B203">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A204" s="1">
         <v>202</v>
       </c>
-      <c r="B204" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B204">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A205" s="1">
         <v>203</v>
       </c>
-      <c r="B205" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B205">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A206" s="1">
         <v>204</v>
       </c>
-      <c r="B206" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B206">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A207" s="1">
         <v>205</v>
       </c>
-      <c r="B207" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B207">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A208" s="1">
         <v>206</v>
       </c>
-      <c r="B208" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B208">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A209" s="1">
         <v>207</v>
       </c>
-      <c r="B209" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B209">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A210" s="1">
         <v>208</v>
       </c>
-      <c r="B210" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B210">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A211" s="1">
         <v>209</v>
       </c>
-      <c r="B211" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B211">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A212" s="1">
         <v>210</v>
       </c>
-      <c r="B212" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B212">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A213" s="1">
         <v>211</v>
       </c>
-      <c r="B213" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B213">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A214" s="1">
         <v>212</v>
       </c>
-      <c r="B214" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B214">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A215" s="1">
         <v>213</v>
       </c>
-      <c r="B215" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B215">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A216" s="1">
         <v>214</v>
       </c>
-      <c r="B216" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B216">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A217" s="1">
         <v>215</v>
       </c>
-      <c r="B217" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B217">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A218" s="1">
         <v>216</v>
       </c>
-      <c r="B218" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B218">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A219" s="1">
         <v>217</v>
       </c>
-      <c r="B219" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B219">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A220" s="1">
         <v>218</v>
       </c>
-      <c r="B220" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B220">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A221" s="1">
         <v>219</v>
       </c>
-      <c r="B221" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B221">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A222" s="1">
         <v>220</v>
       </c>
-      <c r="B222" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B222">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A223" s="1">
         <v>221</v>
       </c>
-      <c r="B223" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B223">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A224" s="1">
         <v>222</v>
       </c>
-      <c r="B224" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B224">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A225" s="1">
         <v>223</v>
       </c>
-      <c r="B225" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B225">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A226" s="1">
         <v>224</v>
       </c>
-      <c r="B226" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B226">
+        <v>2898</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A227" s="1">
         <v>225</v>
       </c>
-      <c r="B227" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B227">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A228" s="1">
         <v>226</v>
       </c>
-      <c r="B228" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B228">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A229" s="1">
         <v>227</v>
       </c>
-      <c r="B229" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B229">
+        <v>1683</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A230" s="1">
         <v>228</v>
       </c>
-      <c r="B230" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B230">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A231" s="1">
         <v>229</v>
       </c>
-      <c r="B231" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B231">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A232" s="1">
         <v>230</v>
       </c>
-      <c r="B232" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B232">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A233" s="1">
         <v>231</v>
       </c>
-      <c r="B233" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B233">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A234" s="1">
         <v>232</v>
       </c>
-      <c r="B234" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B234">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A235" s="1">
         <v>233</v>
       </c>
-      <c r="B235" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B235">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A236" s="1">
         <v>234</v>
       </c>
-      <c r="B236" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B236">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A237" s="1">
         <v>235</v>
       </c>
-      <c r="B237" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B237">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A238" s="1">
         <v>236</v>
       </c>
-      <c r="B238" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B238">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A239" s="1">
         <v>237</v>
       </c>
-      <c r="B239" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B239">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A240" s="1">
         <v>238</v>
       </c>
-      <c r="B240" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B240">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A241" s="1">
         <v>239</v>
       </c>
-      <c r="B241" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B241">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A242" s="1">
         <v>240</v>
       </c>
-      <c r="B242" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B242">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A243" s="1">
         <v>241</v>
       </c>
-      <c r="B243" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B243">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A244" s="1">
         <v>242</v>
       </c>
-      <c r="B244" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B244">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A245" s="1">
         <v>243</v>
       </c>
-      <c r="B245" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B245">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A246" s="1">
         <v>244</v>
       </c>
-      <c r="B246" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B246">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A247" s="1">
         <v>245</v>
       </c>
-      <c r="B247" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B247">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A248" s="1">
         <v>246</v>
       </c>
-      <c r="B248" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B248">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A249" s="1">
         <v>247</v>
       </c>
-      <c r="B249" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B249">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A250" s="1">
         <v>248</v>
       </c>
-      <c r="B250" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B250">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A251" s="1">
         <v>249</v>
       </c>
-      <c r="B251" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B251">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A252" s="1">
         <v>250</v>
       </c>
-      <c r="B252" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B252">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A253" s="1">
         <v>251</v>
       </c>
-      <c r="B253" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B253">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A254" s="1">
         <v>252</v>
       </c>
-      <c r="B254" s="1">
+      <c r="B254">
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A255" s="1">
         <v>253</v>
       </c>
-      <c r="B255" s="1">
+      <c r="B255">
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A256" s="1">
         <v>254</v>
       </c>
-      <c r="B256" s="1">
+      <c r="B256">
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A257" s="1">
         <v>255</v>
       </c>
-      <c r="B257" s="1">
+      <c r="B257">
         <v>0</v>
       </c>
     </row>
@@ -4226,7 +4242,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4238,7 +4254,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>